<commit_message>
Update Hướng dẫn sử dụng phần mềm và các Testcase của phần mềm.xlsx
</commit_message>
<xml_diff>
--- a/Hướng dẫn sử dụng phần mềm và các Testcase của phần mềm.xlsx
+++ b/Hướng dẫn sử dụng phần mềm và các Testcase của phần mềm.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Create Date</t>
   </si>
@@ -72,27 +72,12 @@
     <t>Testcase</t>
   </si>
   <si>
-    <t xml:space="preserve">Cộng 1 chuỗi s1 có n số với 1 chuỗi s2 có n + j số </t>
-  </si>
-  <si>
     <t>Đã hoàn thành</t>
   </si>
   <si>
-    <t xml:space="preserve">Cộng 1 chuỗi s1 có n+j số với 1 chuỗi s2 có n số </t>
-  </si>
-  <si>
-    <t>Cộng 2 chuỗi số có độ dài bằng nhau</t>
-  </si>
-  <si>
-    <t>Kiểm tra xem 2 chuỗi số có chứa chữ hay không</t>
-  </si>
-  <si>
     <t>Kiểm tra xem 2 chuỗi số có chứa kí tự đặc biệt hay không</t>
   </si>
   <si>
-    <t>Kiểm tra xem 2 chuỗi số có chứa số âm hay không</t>
-  </si>
-  <si>
     <t>Hướng dẫn sử dụng phần mềm</t>
   </si>
   <si>
@@ -130,12 +115,6 @@
   </si>
   <si>
     <t>ThanhDuyLuu</t>
-  </si>
-  <si>
-    <t>Kiểm tra xem 2 chuổi có rổng hay không</t>
-  </si>
-  <si>
-    <t>Dã hoàn thành</t>
   </si>
   <si>
     <t>Nhâp số thứ nhất vào ô bên cạnh chữ "Enter First Number"</t>
@@ -229,6 +208,18 @@
   </si>
   <si>
     <t>cách cài đặt cmd:</t>
+  </si>
+  <si>
+    <t>Cộng 2 chuổi có độ dài bằng nhau và trong khi cộng không có số dư</t>
+  </si>
+  <si>
+    <t>Cộng 2 chuổi có độ dài bằng nhau và  trong khi cộng có số dư</t>
+  </si>
+  <si>
+    <t>Cộng 1 chuỗi s1 có n số với 1 chuỗi s2 có n +j số trong khi cộng có số dư</t>
+  </si>
+  <si>
+    <t>Cộng 1 chuỗi s1 có n + j số với 1 chuỗi s2 có n số trong khi cộng có số dư</t>
   </si>
 </sst>
 </file>
@@ -1119,6 +1110,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="24" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1235,15 +1235,6 @@
     </xf>
     <xf numFmtId="15" fontId="27" fillId="0" borderId="33" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1690,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:AC18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
@@ -1700,188 +1691,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="15" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="32" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="34"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="37"/>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="35" t="s">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="36"/>
-      <c r="AI2" s="36"/>
-      <c r="AJ2" s="37"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="40"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="42" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="39" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="50" t="s">
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="51"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="54"/>
       <c r="W3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="54" t="s">
+      <c r="Z3" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="55"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="58"/>
       <c r="AD3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AE3" s="5"/>
       <c r="AF3" s="6"/>
-      <c r="AG3" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="57"/>
-      <c r="AJ3" s="58"/>
+      <c r="AG3" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH3" s="60"/>
+      <c r="AI3" s="60"/>
+      <c r="AJ3" s="61"/>
     </row>
     <row r="4" spans="1:36" ht="15" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="53"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="56"/>
       <c r="W4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="60"/>
+      <c r="Z4" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="63"/>
       <c r="AD4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AE4" s="7"/>
       <c r="AF4" s="8"/>
-      <c r="AG4" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="58"/>
+      <c r="AG4" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH4" s="60"/>
+      <c r="AI4" s="60"/>
+      <c r="AJ4" s="61"/>
     </row>
     <row r="5" spans="1:36" ht="15.75">
       <c r="A5" s="10">
@@ -2011,7 +2002,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -2053,7 +2044,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -2095,7 +2086,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -2216,42 +2207,42 @@
       <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="61"/>
-      <c r="S14" s="61"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="61"/>
-      <c r="AD14" s="17"/>
-      <c r="AE14" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF14" s="61"/>
-      <c r="AG14" s="61"/>
-      <c r="AH14" s="61"/>
-      <c r="AI14" s="61"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="23"/>
+      <c r="AI14" s="23"/>
       <c r="AJ14" s="17"/>
     </row>
     <row r="15" spans="1:36">
@@ -2259,252 +2250,240 @@
       <c r="C15" s="17">
         <v>2</v>
       </c>
-      <c r="D15" s="61" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="61"/>
-      <c r="Y15" s="61"/>
-      <c r="Z15" s="61"/>
-      <c r="AA15" s="61"/>
-      <c r="AB15" s="61"/>
-      <c r="AC15" s="61"/>
+      <c r="D15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
       <c r="AD15" s="17"/>
-      <c r="AE15" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF15" s="61"/>
-      <c r="AG15" s="61"/>
-      <c r="AH15" s="61"/>
-      <c r="AI15" s="61"/>
+      <c r="AE15" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF15" s="23"/>
+      <c r="AG15" s="23"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="23"/>
     </row>
     <row r="16" spans="1:36">
       <c r="B16" s="9"/>
       <c r="C16" s="17">
         <v>3</v>
       </c>
-      <c r="D16" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="61"/>
-      <c r="S16" s="61"/>
-      <c r="T16" s="61"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="61"/>
-      <c r="W16" s="61"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
+      <c r="D16" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="23"/>
       <c r="AD16" s="17"/>
-      <c r="AE16" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF16" s="61"/>
-      <c r="AG16" s="61"/>
-      <c r="AH16" s="61"/>
-      <c r="AI16" s="61"/>
+      <c r="AE16" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF16" s="23"/>
+      <c r="AG16" s="23"/>
+      <c r="AH16" s="23"/>
+      <c r="AI16" s="23"/>
     </row>
     <row r="17" spans="1:36">
       <c r="B17" s="9"/>
       <c r="C17" s="17">
         <v>4</v>
       </c>
-      <c r="D17" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="61"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
+      <c r="D17" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
       <c r="AD17" s="17"/>
-      <c r="AE17" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF17" s="61"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
+      <c r="AE17" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="23"/>
+      <c r="AH17" s="23"/>
+      <c r="AI17" s="23"/>
     </row>
     <row r="18" spans="1:36" ht="15" customHeight="1">
       <c r="B18" s="9"/>
       <c r="C18" s="17">
         <v>5</v>
       </c>
-      <c r="D18" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="R18" s="61"/>
-      <c r="S18" s="61"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="61"/>
-      <c r="AA18" s="61"/>
-      <c r="AB18" s="61"/>
-      <c r="AC18" s="61"/>
+      <c r="D18" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="23"/>
       <c r="AD18" s="17"/>
-      <c r="AE18" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF18" s="61"/>
-      <c r="AG18" s="61"/>
-      <c r="AH18" s="61"/>
-      <c r="AI18" s="61"/>
+      <c r="AE18" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="23"/>
+      <c r="AH18" s="23"/>
+      <c r="AI18" s="23"/>
     </row>
     <row r="19" spans="1:36" ht="15" customHeight="1">
       <c r="B19" s="9"/>
-      <c r="C19" s="17">
-        <v>6</v>
-      </c>
-      <c r="D19" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
-      <c r="Y19" s="61"/>
-      <c r="Z19" s="61"/>
-      <c r="AA19" s="61"/>
-      <c r="AB19" s="61"/>
-      <c r="AC19" s="61"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
       <c r="AD19" s="17"/>
-      <c r="AE19" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF19" s="61"/>
-      <c r="AG19" s="61"/>
-      <c r="AH19" s="61"/>
-      <c r="AI19" s="61"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="23"/>
+      <c r="AI19" s="23"/>
     </row>
     <row r="20" spans="1:36">
       <c r="B20" s="9"/>
-      <c r="C20" s="17">
-        <v>7</v>
-      </c>
-      <c r="D20" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
-      <c r="R20" s="61"/>
-      <c r="S20" s="61"/>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
-      <c r="Z20" s="61"/>
-      <c r="AA20" s="61"/>
-      <c r="AB20" s="61"/>
-      <c r="AC20" s="61"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
       <c r="AD20" s="17"/>
-      <c r="AE20" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF20" s="61"/>
-      <c r="AG20" s="61"/>
-      <c r="AH20" s="61"/>
-      <c r="AI20" s="61"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="23"/>
+      <c r="AH20" s="23"/>
+      <c r="AI20" s="23"/>
     </row>
     <row r="21" spans="1:36">
       <c r="C21" s="14"/>
@@ -2547,7 +2526,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2588,128 +2567,128 @@
       <c r="C24" s="20">
         <v>1</v>
       </c>
-      <c r="D24" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="63"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
-      <c r="Z24" s="63"/>
-      <c r="AA24" s="63"/>
-      <c r="AB24" s="63"/>
-      <c r="AC24" s="63"/>
-      <c r="AD24" s="63"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
+      <c r="D24" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="24"/>
+      <c r="AG24" s="24"/>
+      <c r="AH24" s="24"/>
+      <c r="AI24" s="24"/>
+      <c r="AJ24" s="24"/>
     </row>
     <row r="25" spans="1:36">
       <c r="C25" s="20">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:36">
-      <c r="D26" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="63"/>
-      <c r="L26" s="63"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="63"/>
-      <c r="U26" s="63"/>
-      <c r="V26" s="63"/>
-      <c r="W26" s="63"/>
-      <c r="X26" s="63"/>
-      <c r="Y26" s="63"/>
-      <c r="Z26" s="63"/>
-      <c r="AA26" s="63"/>
-      <c r="AB26" s="63"/>
-      <c r="AC26" s="63"/>
-      <c r="AD26" s="63"/>
-      <c r="AE26" s="63"/>
-      <c r="AF26" s="63"/>
-      <c r="AG26" s="63"/>
-      <c r="AH26" s="63"/>
-      <c r="AI26" s="63"/>
+      <c r="D26" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="24"/>
+      <c r="Z26" s="24"/>
+      <c r="AA26" s="24"/>
+      <c r="AB26" s="24"/>
+      <c r="AC26" s="24"/>
+      <c r="AD26" s="24"/>
+      <c r="AE26" s="24"/>
+      <c r="AF26" s="24"/>
+      <c r="AG26" s="24"/>
+      <c r="AH26" s="24"/>
+      <c r="AI26" s="24"/>
     </row>
     <row r="27" spans="1:36">
       <c r="C27" s="19">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:36">
       <c r="C28" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:36">
       <c r="D29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:36">
       <c r="D30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:36">
       <c r="B31" s="17"/>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:36">
@@ -2718,7 +2697,7 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="3:36">
@@ -2726,34 +2705,34 @@
       <c r="D33" s="18">
         <v>1</v>
       </c>
-      <c r="E33" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="62"/>
-      <c r="T33" s="62"/>
-      <c r="U33" s="62"/>
-      <c r="V33" s="62"/>
-      <c r="W33" s="62"/>
-      <c r="X33" s="62"/>
-      <c r="Y33" s="62"/>
-      <c r="Z33" s="62"/>
-      <c r="AA33" s="62"/>
-      <c r="AB33" s="62"/>
-      <c r="AC33" s="62"/>
-      <c r="AD33" s="62"/>
+      <c r="E33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
       <c r="AE33" s="17"/>
       <c r="AF33" s="17"/>
       <c r="AG33" s="17"/>
@@ -2766,34 +2745,34 @@
       <c r="D34" s="18">
         <v>2</v>
       </c>
-      <c r="E34" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="62"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="62"/>
-      <c r="S34" s="62"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
-      <c r="Y34" s="62"/>
-      <c r="Z34" s="62"/>
-      <c r="AA34" s="62"/>
-      <c r="AB34" s="62"/>
-      <c r="AC34" s="62"/>
-      <c r="AD34" s="62"/>
+      <c r="E34" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="22"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="22"/>
+      <c r="X34" s="22"/>
+      <c r="Y34" s="22"/>
+      <c r="Z34" s="22"/>
+      <c r="AA34" s="22"/>
+      <c r="AB34" s="22"/>
+      <c r="AC34" s="22"/>
+      <c r="AD34" s="22"/>
       <c r="AE34" s="17"/>
       <c r="AF34" s="17"/>
       <c r="AG34" s="17"/>
@@ -2805,65 +2784,46 @@
       <c r="D35" s="18">
         <v>3</v>
       </c>
-      <c r="E35" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="62"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="62"/>
-      <c r="S35" s="62"/>
-      <c r="T35" s="62"/>
-      <c r="U35" s="62"/>
-      <c r="V35" s="62"/>
-      <c r="W35" s="62"/>
-      <c r="X35" s="62"/>
-      <c r="Y35" s="62"/>
-      <c r="Z35" s="62"/>
-      <c r="AA35" s="62"/>
-      <c r="AB35" s="62"/>
-      <c r="AC35" s="62"/>
-      <c r="AD35" s="62"/>
+      <c r="E35" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="22"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="22"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="22"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+      <c r="Z35" s="22"/>
+      <c r="AA35" s="22"/>
+      <c r="AB35" s="22"/>
+      <c r="AC35" s="22"/>
+      <c r="AD35" s="22"/>
     </row>
     <row r="36" spans="3:36">
       <c r="D36" s="21">
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="E34:AD34"/>
-    <mergeCell ref="E35:AD35"/>
-    <mergeCell ref="AE18:AI18"/>
-    <mergeCell ref="D19:AC19"/>
-    <mergeCell ref="AE19:AI19"/>
-    <mergeCell ref="D20:AC20"/>
-    <mergeCell ref="AE20:AI20"/>
-    <mergeCell ref="D24:AJ24"/>
-    <mergeCell ref="D14:AC14"/>
-    <mergeCell ref="AE14:AI14"/>
-    <mergeCell ref="D15:AC15"/>
-    <mergeCell ref="AE15:AI15"/>
-    <mergeCell ref="E33:AD33"/>
-    <mergeCell ref="D16:AC16"/>
-    <mergeCell ref="AE16:AI16"/>
-    <mergeCell ref="D17:AC17"/>
-    <mergeCell ref="AE17:AI17"/>
-    <mergeCell ref="D18:AC18"/>
-    <mergeCell ref="D26:AI26"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="E1:V2"/>
     <mergeCell ref="W1:AJ1"/>
@@ -2876,6 +2836,25 @@
     <mergeCell ref="AG3:AJ3"/>
     <mergeCell ref="Z4:AC4"/>
     <mergeCell ref="AG4:AJ4"/>
+    <mergeCell ref="D14:AC14"/>
+    <mergeCell ref="AE14:AI14"/>
+    <mergeCell ref="D15:AC15"/>
+    <mergeCell ref="AE15:AI15"/>
+    <mergeCell ref="E33:AD33"/>
+    <mergeCell ref="D16:AC16"/>
+    <mergeCell ref="AE16:AI16"/>
+    <mergeCell ref="D17:AC17"/>
+    <mergeCell ref="AE17:AI17"/>
+    <mergeCell ref="D18:AC18"/>
+    <mergeCell ref="D26:AI26"/>
+    <mergeCell ref="E34:AD34"/>
+    <mergeCell ref="E35:AD35"/>
+    <mergeCell ref="AE18:AI18"/>
+    <mergeCell ref="D19:AC19"/>
+    <mergeCell ref="AE19:AI19"/>
+    <mergeCell ref="D20:AC20"/>
+    <mergeCell ref="AE20:AI20"/>
+    <mergeCell ref="D24:AJ24"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.31496062992125984" top="0.39370078740157483" bottom="0.31496062992125984" header="0.15748031496062992" footer="0.15748031496062992"/>
   <pageSetup paperSize="8" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>